<commit_message>
add function to add allocation section
</commit_message>
<xml_diff>
--- a/src/main/resources/AzubiDaten.xlsx
+++ b/src/main/resources/AzubiDaten.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Name, Vorname</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>FIAE</t>
+  </si>
+  <si>
+    <t>Praktikumsabschnitt</t>
   </si>
 </sst>
 </file>
@@ -370,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -383,9 +386,10 @@
     <col min="3" max="3" width="28" customWidth="1"/>
     <col min="6" max="6" width="14.453125" customWidth="1"/>
     <col min="7" max="7" width="17.90625" customWidth="1"/>
+    <col min="8" max="8" width="23.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -407,8 +411,11 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -429,6 +436,9 @@
       </c>
       <c r="G2" s="2">
         <v>43557</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>